<commit_message>
Asignación de las tareas semana #1 ciclo #3
</commit_message>
<xml_diff>
--- a/tspi/ciclo-2/20105914.xlsx
+++ b/tspi/ciclo-2/20105914.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="9660" yWindow="-45" windowWidth="9540" windowHeight="7365" tabRatio="400" activeTab="2"/>
+    <workbookView xWindow="9660" yWindow="-45" windowWidth="9540" windowHeight="7365" tabRatio="400"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t>Id</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>Elaborar el reporte de cierre del ciclo #2 de TSPi.</t>
+  </si>
+  <si>
+    <t>Physical Data Model</t>
   </si>
 </sst>
 </file>
@@ -689,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:ALY23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -17555,10 +17558,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -17654,68 +17657,75 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="4">
         <f>SUMIF(logt!$G:$G,A8,logt!$F:$F)/60</f>
-        <v>0.48333333333333334</v>
+        <v>1.8333333333333333</v>
       </c>
       <c r="C8" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="12" customFormat="1">
-      <c r="A9" s="31">
-        <v>41</v>
+    <row r="9" spans="1:3">
+      <c r="A9" s="4">
+        <v>38</v>
       </c>
       <c r="B9" s="4">
         <f>SUMIF(logt!$G:$G,A9,logt!$F:$F)/60</f>
-        <v>1.25</v>
-      </c>
-      <c r="C9" s="31">
+        <v>0.48333333333333334</v>
+      </c>
+      <c r="C9" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="4">
-        <v>42</v>
+    <row r="10" spans="1:3" s="12" customFormat="1">
+      <c r="A10" s="31">
+        <v>41</v>
       </c>
       <c r="B10" s="4">
         <f>SUMIF(logt!$G:$G,A10,logt!$F:$F)/60</f>
-        <v>4.416666666666667</v>
-      </c>
-      <c r="C10" s="4">
-        <v>4</v>
+        <v>1.25</v>
+      </c>
+      <c r="C10" s="31">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="4">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="4">
         <f>SUMIF(logt!$G:$G,A11,logt!$F:$F)/60</f>
-        <v>1.3333333333333333</v>
+        <v>4.416666666666667</v>
       </c>
       <c r="C11" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="4">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B12" s="4">
         <f>SUMIF(logt!$G:$G,A12,logt!$F:$F)/60</f>
-        <v>0.95</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="C12" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+      <c r="A13" s="4">
+        <v>45</v>
+      </c>
+      <c r="B13" s="4">
+        <f>SUMIF(logt!$G:$G,A13,logt!$F:$F)/60</f>
+        <v>0.95</v>
+      </c>
+      <c r="C13" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="4"/>
@@ -17742,6 +17752,11 @@
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -17754,10 +17769,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:K3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="12.75"/>
@@ -17815,7 +17830,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="16">
-        <f t="shared" ref="F2:F13" si="0">((HOUR(D2)-HOUR(C2))*60)+(MINUTE(D2)-MINUTE(C2))-E2</f>
+        <f t="shared" ref="F2:F14" si="0">((HOUR(D2)-HOUR(C2))*60)+(MINUTE(D2)-MINUTE(C2))-E2</f>
         <v>30</v>
       </c>
       <c r="G2" s="4">
@@ -18043,92 +18058,110 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="22">
-        <v>41938</v>
+        <v>41935</v>
       </c>
       <c r="B11" s="28">
         <v>5</v>
       </c>
       <c r="C11" s="23">
+        <v>0.625</v>
+      </c>
+      <c r="D11" s="23">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E11" s="30">
+        <v>10</v>
+      </c>
+      <c r="F11" s="24">
+        <v>110</v>
+      </c>
+      <c r="G11" s="4">
+        <v>37</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="22">
+        <v>41938</v>
+      </c>
+      <c r="B12" s="28">
+        <v>5</v>
+      </c>
+      <c r="C12" s="23">
         <v>0.41805555555555557</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D12" s="23">
         <v>0.44027777777777777</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E12" s="30">
         <v>0</v>
       </c>
-      <c r="F11" s="24">
+      <c r="F12" s="24">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G12" s="4">
         <v>43</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H12" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="25.5">
-      <c r="A12" s="22">
+    <row r="13" spans="1:8" ht="25.5">
+      <c r="A13" s="22">
         <v>41938</v>
       </c>
-      <c r="B12" s="28">
+      <c r="B13" s="28">
         <v>5</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C13" s="23">
         <v>0.44166666666666665</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D13" s="23">
         <v>0.46180555555555558</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E13" s="30">
         <v>0</v>
       </c>
-      <c r="F12" s="24">
+      <c r="F13" s="24">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G13" s="4">
         <v>38</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H13" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="22">
+    <row r="14" spans="1:8">
+      <c r="A14" s="22">
         <v>41938</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B14" s="28">
         <v>5</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C14" s="23">
         <v>0.46527777777777773</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D14" s="23">
         <v>0.50486111111111109</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E14" s="30">
         <v>0</v>
       </c>
-      <c r="F13" s="24">
+      <c r="F14" s="24">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G14" s="4">
         <v>45</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H14" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="22"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="24"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="22"/>
@@ -18138,34 +18171,34 @@
       <c r="E15" s="30"/>
       <c r="F15" s="24"/>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="22"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="24"/>
+    <row r="17" spans="1:8">
+      <c r="F17" s="16"/>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="22"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="24"/>
+    <row r="18" spans="1:8" s="12" customFormat="1">
+      <c r="A18" s="19"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="F19" s="16"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="24"/>
     </row>
-    <row r="20" spans="1:8" s="12" customFormat="1">
-      <c r="A20" s="19"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
+    <row r="20" spans="1:8">
+      <c r="A20" s="22"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="24"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="22"/>
@@ -18279,24 +18312,8 @@
       <c r="E34" s="30"/>
       <c r="F34" s="24"/>
     </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="22"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="24"/>
-    </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="22"/>
-      <c r="B36" s="28"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="24"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="F38" s="16"/>
+      <c r="F36" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>